<commit_message>
Cambio en tiempos de estudio
</commit_message>
<xml_diff>
--- a/Planeacion.xlsx
+++ b/Planeacion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\UdeA\Info ii\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\UdeA\Info ii\Actividad 2 Planeacion mes GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053F6597-B5FB-4591-86B0-0C883D43CAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21CA7CA-E3FB-4F04-8428-A129C21FBB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B8AEF582-178D-4707-94F7-F655300FE6C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="32">
   <si>
     <t xml:space="preserve">Domingo </t>
   </si>
@@ -112,6 +112,24 @@
   </si>
   <si>
     <t xml:space="preserve">Asesoria Calculo vectorial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">asesoria calculo vectorial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">asesoria probabilidad y estadistica </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cita </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiempo estudio calculo vectorial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiempo estudio probabilidad y estadistica </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cita </t>
   </si>
 </sst>
 </file>
@@ -303,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -351,27 +369,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -381,23 +417,29 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -715,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42C7FCB-557D-4E95-86EC-B3EBDEE8C635}">
   <dimension ref="A3:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,22 +870,22 @@
         <v>0.33333333333333298</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="18" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -852,12 +894,12 @@
         <v>0.375</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="32"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="19"/>
-      <c r="F8" s="32"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="17"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
@@ -867,39 +909,39 @@
         <v>15</v>
       </c>
       <c r="C9" s="22"/>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="23"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="23"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="2"/>
       <c r="D11" s="10" t="s">
         <v>15</v>
@@ -946,19 +988,19 @@
       <c r="B13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="30" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="25" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="25" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="14" t="s">
@@ -970,16 +1012,16 @@
         <v>0.625</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="25"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="30"/>
+      <c r="E14" s="25"/>
       <c r="F14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="17" t="s">
+      <c r="G14" s="25"/>
+      <c r="H14" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -988,20 +1030,20 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="20" t="s">
+      <c r="C15" s="32"/>
+      <c r="D15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="23" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
@@ -1012,29 +1054,29 @@
         <v>24</v>
       </c>
       <c r="D16" s="22"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="17"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>0.75</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="19"/>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="2"/>
@@ -1046,13 +1088,13 @@
       <c r="B18" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="14" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="19"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1074,7 +1116,7 @@
       <c r="F19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="17"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="8" t="s">
         <v>20</v>
       </c>
@@ -1109,25 +1151,25 @@
       <c r="A21" s="4">
         <v>0.91666666666666696</v>
       </c>
-      <c r="B21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="27" t="s">
+      <c r="B21" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="26" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1135,25 +1177,25 @@
       <c r="A22" s="4">
         <v>0.95833333333333404</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>1</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
@@ -1268,19 +1310,19 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="19"/>
-      <c r="D29" s="32" t="s">
+      <c r="D29" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="32" t="s">
+      <c r="F29" s="18" t="s">
         <v>8</v>
       </c>
       <c r="G29" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1290,11 +1332,11 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="19"/>
-      <c r="D30" s="32"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="19"/>
-      <c r="F30" s="32"/>
+      <c r="F30" s="18"/>
       <c r="G30" s="19"/>
-      <c r="H30" s="17"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="31" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
@@ -1304,39 +1346,39 @@
         <v>15</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G31" s="18" t="s">
+      <c r="G31" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="17"/>
+      <c r="H31" s="20"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="23"/>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>0.5</v>
       </c>
-      <c r="B33" s="23"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="2"/>
       <c r="D33" s="10" t="s">
         <v>15</v>
@@ -1381,17 +1423,17 @@
       <c r="B35" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="25" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="2"/>
-      <c r="G35" s="30" t="s">
+      <c r="G35" s="25" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="14" t="s">
@@ -1403,14 +1445,14 @@
         <v>0.625</v>
       </c>
       <c r="B36" s="14"/>
-      <c r="C36" s="21"/>
+      <c r="C36" s="29"/>
       <c r="D36" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="30"/>
+      <c r="E36" s="25"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="17" t="s">
+      <c r="G36" s="25"/>
+      <c r="H36" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1421,16 +1463,16 @@
       <c r="B37" s="2"/>
       <c r="C37" s="22"/>
       <c r="D37" s="19"/>
-      <c r="E37" s="18" t="s">
+      <c r="E37" s="23" t="s">
         <v>23</v>
       </c>
       <c r="F37" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G37" s="31" t="s">
+      <c r="G37" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="17"/>
+      <c r="H37" s="20"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
@@ -1441,29 +1483,29 @@
         <v>24</v>
       </c>
       <c r="D38" s="19"/>
-      <c r="E38" s="18"/>
+      <c r="E38" s="23"/>
       <c r="F38" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G38" s="31"/>
-      <c r="H38" s="17"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="20"/>
     </row>
     <row r="39" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>0.75</v>
       </c>
       <c r="B39" s="2"/>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F39" s="19"/>
-      <c r="G39" s="17" t="s">
+      <c r="G39" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H39" s="2"/>
@@ -1475,13 +1517,13 @@
       <c r="B40" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="18"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="23"/>
       <c r="E40" s="14" t="s">
         <v>24</v>
       </c>
       <c r="F40" s="19"/>
-      <c r="G40" s="17"/>
+      <c r="G40" s="20"/>
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -1503,7 +1545,7 @@
       <c r="F41" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G41" s="17"/>
+      <c r="G41" s="20"/>
       <c r="H41" s="8" t="s">
         <v>20</v>
       </c>
@@ -1538,25 +1580,25 @@
       <c r="A43" s="4">
         <v>0.91666666666666696</v>
       </c>
-      <c r="B43" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C43" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F43" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G43" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" s="27" t="s">
+      <c r="B43" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="26" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1564,25 +1606,25 @@
       <c r="A44" s="4">
         <v>0.95833333333333404</v>
       </c>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>1</v>
       </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="15"/>
@@ -1673,9 +1715,7 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="B50" s="2"/>
-      <c r="C50" s="19" t="s">
-        <v>22</v>
-      </c>
+      <c r="C50" s="36"/>
       <c r="D50" s="10" t="s">
         <v>15</v>
       </c>
@@ -1695,20 +1735,22 @@
         <v>0.33333333333333298</v>
       </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="32" t="s">
+      <c r="C51" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="32" t="s">
+      <c r="F51" s="18" t="s">
         <v>8</v>
       </c>
       <c r="G51" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H51" s="17" t="s">
+      <c r="H51" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1717,12 +1759,12 @@
         <v>0.375</v>
       </c>
       <c r="B52" s="2"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="32"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="18"/>
       <c r="E52" s="19"/>
-      <c r="F52" s="32"/>
+      <c r="F52" s="18"/>
       <c r="G52" s="19"/>
-      <c r="H52" s="17"/>
+      <c r="H52" s="20"/>
     </row>
     <row r="53" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
@@ -1731,41 +1773,42 @@
       <c r="B53" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="17" t="s">
+      <c r="C53" s="22"/>
+      <c r="D53" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E53" s="18" t="s">
+      <c r="E53" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F53" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G53" s="18" t="s">
+      <c r="G53" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H53" s="17"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H53" s="20"/>
+    </row>
+    <row r="54" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B54" s="23" t="s">
+      <c r="B54" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="18"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="23"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
         <v>0.5</v>
       </c>
-      <c r="B55" s="23"/>
-      <c r="C55" s="2"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="31" t="s">
+        <v>29</v>
+      </c>
       <c r="D55" s="10" t="s">
         <v>15</v>
       </c>
@@ -1785,16 +1828,14 @@
       <c r="B56" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C56" s="32"/>
       <c r="D56" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F56" s="2"/>
+      <c r="F56" s="39"/>
       <c r="G56" s="8" t="s">
         <v>20</v>
       </c>
@@ -1809,89 +1850,89 @@
       <c r="B57" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E57" s="30" t="s">
+      <c r="C57" s="36"/>
+      <c r="D57" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F57" s="2"/>
-      <c r="G57" s="30" t="s">
+      <c r="F57" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G57" s="25" t="s">
         <v>13</v>
       </c>
       <c r="H57" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
         <v>0.625</v>
       </c>
-      <c r="B58" s="14"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E58" s="30"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="30"/>
-      <c r="H58" s="17" t="s">
+      <c r="B58" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="36"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G59" s="31" t="s">
+      <c r="B59" s="34"/>
+      <c r="C59" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="36"/>
+      <c r="F59" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H59" s="17"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H59" s="20"/>
+    </row>
+    <row r="60" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
         <v>0.70833333333333404</v>
       </c>
-      <c r="B60" s="2"/>
-      <c r="C60" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D60" s="19"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G60" s="31"/>
-      <c r="H60" s="17"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G60" s="24"/>
+      <c r="H60" s="20"/>
     </row>
     <row r="61" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
         <v>0.75</v>
       </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D61" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F61" s="19"/>
-      <c r="G61" s="17" t="s">
+      <c r="B61" s="34"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F61" s="36"/>
+      <c r="G61" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H61" s="2"/>
@@ -1900,28 +1941,24 @@
       <c r="A62" s="4">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B62" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" s="17"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F62" s="19"/>
-      <c r="G62" s="17"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F62" s="36"/>
+      <c r="G62" s="20"/>
       <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="4">
         <v>0.83333333333333404</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="B63" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="37"/>
       <c r="D63" s="8" t="s">
         <v>20</v>
       </c>
@@ -1931,7 +1968,7 @@
       <c r="F63" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G63" s="17"/>
+      <c r="G63" s="20"/>
       <c r="H63" s="8" t="s">
         <v>20</v>
       </c>
@@ -1943,9 +1980,7 @@
       <c r="B64" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="C64" s="37"/>
       <c r="D64" s="7" t="s">
         <v>18</v>
       </c>
@@ -1966,25 +2001,25 @@
       <c r="A65" s="4">
         <v>0.91666666666666696</v>
       </c>
-      <c r="B65" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D65" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E65" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F65" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G65" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H65" s="27" t="s">
+      <c r="B65" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G65" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H65" s="26" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1992,25 +2027,25 @@
       <c r="A66" s="4">
         <v>0.95833333333333404</v>
       </c>
-      <c r="B66" s="28"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28"/>
-      <c r="G66" s="28"/>
-      <c r="H66" s="28"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="27"/>
+      <c r="H66" s="27"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="4">
         <v>1</v>
       </c>
-      <c r="B67" s="29"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
-      <c r="G67" s="29"/>
-      <c r="H67" s="29"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="15"/>
@@ -2124,19 +2159,19 @@
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="19"/>
-      <c r="D73" s="32" t="s">
+      <c r="D73" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F73" s="32" t="s">
+      <c r="F73" s="18" t="s">
         <v>8</v>
       </c>
       <c r="G73" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H73" s="17" t="s">
+      <c r="H73" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2146,11 +2181,11 @@
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="19"/>
-      <c r="D74" s="32"/>
+      <c r="D74" s="18"/>
       <c r="E74" s="19"/>
-      <c r="F74" s="32"/>
+      <c r="F74" s="18"/>
       <c r="G74" s="19"/>
-      <c r="H74" s="17"/>
+      <c r="H74" s="20"/>
     </row>
     <row r="75" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="4">
@@ -2160,44 +2195,46 @@
         <v>15</v>
       </c>
       <c r="C75" s="2"/>
-      <c r="D75" s="17" t="s">
+      <c r="D75" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E75" s="18" t="s">
+      <c r="E75" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F75" s="17" t="s">
+      <c r="F75" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G75" s="18" t="s">
+      <c r="G75" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H75" s="17"/>
+      <c r="H75" s="20"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B76" s="23" t="s">
+      <c r="B76" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C76" s="2"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="18"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="23"/>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="4">
         <v>0.5</v>
       </c>
-      <c r="B77" s="23"/>
+      <c r="B77" s="17"/>
       <c r="C77" s="2"/>
       <c r="D77" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E77" s="12"/>
+      <c r="E77" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="F77" s="8" t="s">
         <v>20</v>
       </c>
@@ -2219,7 +2256,7 @@
       <c r="D78" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E78" s="8" t="s">
+      <c r="E78" s="40" t="s">
         <v>20</v>
       </c>
       <c r="F78" s="2"/>
@@ -2237,17 +2274,17 @@
       <c r="B79" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="C79" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D79" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E79" s="30" t="s">
+      <c r="E79" s="25" t="s">
         <v>13</v>
       </c>
       <c r="F79" s="2"/>
-      <c r="G79" s="30" t="s">
+      <c r="G79" s="25" t="s">
         <v>13</v>
       </c>
       <c r="H79" s="14" t="s">
@@ -2259,14 +2296,14 @@
         <v>0.625</v>
       </c>
       <c r="B80" s="14"/>
-      <c r="C80" s="21"/>
+      <c r="C80" s="29"/>
       <c r="D80" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E80" s="30"/>
+      <c r="E80" s="25"/>
       <c r="F80" s="2"/>
-      <c r="G80" s="30"/>
-      <c r="H80" s="17" t="s">
+      <c r="G80" s="25"/>
+      <c r="H80" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2277,16 +2314,16 @@
       <c r="B81" s="2"/>
       <c r="C81" s="22"/>
       <c r="D81" s="19"/>
-      <c r="E81" s="18" t="s">
+      <c r="E81" s="23" t="s">
         <v>23</v>
       </c>
       <c r="F81" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G81" s="31" t="s">
+      <c r="G81" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H81" s="17"/>
+      <c r="H81" s="20"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="4">
@@ -2297,29 +2334,29 @@
         <v>24</v>
       </c>
       <c r="D82" s="19"/>
-      <c r="E82" s="18"/>
+      <c r="E82" s="23"/>
       <c r="F82" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G82" s="31"/>
-      <c r="H82" s="17"/>
+      <c r="G82" s="24"/>
+      <c r="H82" s="20"/>
     </row>
     <row r="83" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="4">
         <v>0.75</v>
       </c>
       <c r="B83" s="2"/>
-      <c r="C83" s="17" t="s">
+      <c r="C83" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D83" s="18" t="s">
+      <c r="D83" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F83" s="19"/>
-      <c r="G83" s="17" t="s">
+      <c r="G83" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H83" s="2"/>
@@ -2331,13 +2368,13 @@
       <c r="B84" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C84" s="17"/>
-      <c r="D84" s="18"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="23"/>
       <c r="E84" s="14" t="s">
         <v>24</v>
       </c>
       <c r="F84" s="19"/>
-      <c r="G84" s="17"/>
+      <c r="G84" s="20"/>
       <c r="H84" s="2"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
@@ -2359,7 +2396,7 @@
       <c r="F85" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G85" s="17"/>
+      <c r="G85" s="20"/>
       <c r="H85" s="8" t="s">
         <v>20</v>
       </c>
@@ -2394,25 +2431,25 @@
       <c r="A87" s="4">
         <v>0.91666666666666696</v>
       </c>
-      <c r="B87" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C87" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D87" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E87" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F87" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G87" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H87" s="27" t="s">
+      <c r="B87" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D87" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E87" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F87" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G87" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H87" s="26" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2420,59 +2457,83 @@
       <c r="A88" s="4">
         <v>0.95833333333333404</v>
       </c>
-      <c r="B88" s="28"/>
-      <c r="C88" s="28"/>
-      <c r="D88" s="28"/>
-      <c r="E88" s="28"/>
-      <c r="F88" s="28"/>
-      <c r="G88" s="28"/>
-      <c r="H88" s="28"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="27"/>
+      <c r="G88" s="27"/>
+      <c r="H88" s="27"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="4">
         <v>1</v>
       </c>
-      <c r="B89" s="29"/>
-      <c r="C89" s="29"/>
-      <c r="D89" s="29"/>
-      <c r="E89" s="29"/>
-      <c r="F89" s="29"/>
-      <c r="G89" s="29"/>
-      <c r="H89" s="29"/>
+      <c r="B89" s="28"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="28"/>
+      <c r="G89" s="28"/>
+      <c r="H89" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="116">
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="G37:G38"/>
+  <mergeCells count="115">
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="H80:H82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="F82:F84"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="H73:H75"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="H58:H60"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H65:H67"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="C87:C89"/>
+    <mergeCell ref="D87:D89"/>
+    <mergeCell ref="E87:E89"/>
+    <mergeCell ref="F87:F89"/>
+    <mergeCell ref="G87:G89"/>
+    <mergeCell ref="H87:H89"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="D80:D82"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="H43:H45"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="H51:H53"/>
     <mergeCell ref="G83:G85"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="C21:C23"/>
@@ -2497,67 +2558,42 @@
     <mergeCell ref="F65:F67"/>
     <mergeCell ref="G65:G67"/>
     <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="H65:H67"/>
-    <mergeCell ref="B87:B89"/>
-    <mergeCell ref="C87:C89"/>
-    <mergeCell ref="D87:D89"/>
-    <mergeCell ref="E87:E89"/>
-    <mergeCell ref="F87:F89"/>
-    <mergeCell ref="G87:G89"/>
-    <mergeCell ref="H87:H89"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="D80:D82"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="H43:H45"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="G37:G38"/>
     <mergeCell ref="D53:D54"/>
     <mergeCell ref="F53:F54"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="H58:H60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F60:F62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="H80:H82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="F82:F84"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="C72:C74"/>
-    <mergeCell ref="H73:H75"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="H36:H38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="D17:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>